<commit_message>
update room locations to match with json
</commit_message>
<xml_diff>
--- a/RoomLocation.xlsx
+++ b/RoomLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rushil\Desktop\Projects\MapMyJIIT\BunkMyJIIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508698D3-11CA-4137-848B-CFFA85DD0D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E12A6E1-0C86-4E4D-95B4-E30BC2C56943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{68250A3F-BA9E-42BE-ABA5-2F7120A1BC65}"/>
   </bookViews>
@@ -36,54 +36,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="129">
   <si>
-    <t>G-1</t>
-  </si>
-  <si>
     <t>ABB-I</t>
   </si>
   <si>
     <t>Ground Floor</t>
   </si>
   <si>
-    <t>G-2</t>
-  </si>
-  <si>
-    <t>G-3</t>
-  </si>
-  <si>
-    <t>G-4</t>
-  </si>
-  <si>
-    <t>G-5</t>
-  </si>
-  <si>
-    <t>G-6</t>
-  </si>
-  <si>
-    <t>G-7</t>
-  </si>
-  <si>
-    <t>G-8</t>
-  </si>
-  <si>
-    <t>G-9</t>
-  </si>
-  <si>
-    <t>G-10</t>
-  </si>
-  <si>
     <t>ABB-II</t>
   </si>
   <si>
-    <t>G-11</t>
-  </si>
-  <si>
-    <t>G-12</t>
-  </si>
-  <si>
-    <t>G-13</t>
-  </si>
-  <si>
     <t>LT-1</t>
   </si>
   <si>
@@ -144,54 +105,9 @@
     <t>F9</t>
   </si>
   <si>
-    <t>F-10</t>
-  </si>
-  <si>
-    <t>CS-1</t>
-  </si>
-  <si>
     <t>Second Floor</t>
   </si>
   <si>
-    <t>CS-2</t>
-  </si>
-  <si>
-    <t>CS-3</t>
-  </si>
-  <si>
-    <t>CS-4</t>
-  </si>
-  <si>
-    <t>CS-5</t>
-  </si>
-  <si>
-    <t>CS-6</t>
-  </si>
-  <si>
-    <t>CS-7</t>
-  </si>
-  <si>
-    <t>CS-8</t>
-  </si>
-  <si>
-    <t>CS-9</t>
-  </si>
-  <si>
-    <t>CS-10</t>
-  </si>
-  <si>
-    <t>CS-12</t>
-  </si>
-  <si>
-    <t>CS-13</t>
-  </si>
-  <si>
-    <t>CS-14</t>
-  </si>
-  <si>
-    <t>CS-15</t>
-  </si>
-  <si>
     <t>CS16</t>
   </si>
   <si>
@@ -279,9 +195,6 @@
     <t>CL304</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3rd floor</t>
-  </si>
-  <si>
     <t>CL306</t>
   </si>
   <si>
@@ -421,13 +334,100 @@
   </si>
   <si>
     <t>5th floor</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>G13</t>
+  </si>
+  <si>
+    <t>CS1</t>
+  </si>
+  <si>
+    <t>CS2</t>
+  </si>
+  <si>
+    <t>CS3</t>
+  </si>
+  <si>
+    <t>CS4</t>
+  </si>
+  <si>
+    <t>CS5</t>
+  </si>
+  <si>
+    <t>CS6</t>
+  </si>
+  <si>
+    <t>CS7</t>
+  </si>
+  <si>
+    <t>CS8</t>
+  </si>
+  <si>
+    <t>CS9</t>
+  </si>
+  <si>
+    <t>CS10</t>
+  </si>
+  <si>
+    <t>CS12</t>
+  </si>
+  <si>
+    <t>CS13</t>
+  </si>
+  <si>
+    <t>CS14</t>
+  </si>
+  <si>
+    <t>CS15</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>3rd floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +492,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -596,7 +602,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,9 +698,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F85D740-A33C-469B-B8A8-5210F9C03359}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,1116 +1045,1124 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
-        <v>10</v>
+      <c r="A10" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>11</v>
+      <c r="A11" s="31" t="s">
+        <v>109</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>13</v>
+      <c r="A12" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>14</v>
+      <c r="A13" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>15</v>
+      <c r="A14" s="31" t="s">
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>1</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>1</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
-        <v>19</v>
+      <c r="A18" s="33" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>20</v>
+      <c r="A19" s="33" t="s">
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C32" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
-        <v>35</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
-        <v>49</v>
+      <c r="A46" s="33" t="s">
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="34" t="s">
-        <v>50</v>
+      <c r="A47" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="34" t="s">
-        <v>51</v>
+      <c r="A48" s="33" t="s">
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="34" t="s">
-        <v>52</v>
+      <c r="A49" s="33" t="s">
+        <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
-        <v>53</v>
+      <c r="A50" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
-        <v>63</v>
+      <c r="A56" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C82" s="26" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C84" s="26" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="15" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="16" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="16" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="16" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="16" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="16" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A36" r:id="rId1" display="CS@" xr:uid="{0B757EAB-3733-4D4D-B261-ABEB1A17B992}"/>
+    <hyperlink ref="A38" r:id="rId2" display="CS@" xr:uid="{0CE276A1-DF7C-4B25-B93D-64B2159E0B7D}"/>
+    <hyperlink ref="A40" r:id="rId3" display="CS@" xr:uid="{34573C36-AD4F-4AEB-9ED8-979E5808F701}"/>
+    <hyperlink ref="A42" r:id="rId4" display="CS@" xr:uid="{3314547A-CD27-4353-9398-D4004A0DF794}"/>
+    <hyperlink ref="A44" r:id="rId5" display="CS@" xr:uid="{1B4A6DFC-E458-4274-812A-E7616A6AFAC5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more room location updates kill me pls
</commit_message>
<xml_diff>
--- a/RoomLocation.xlsx
+++ b/RoomLocation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rushil\Desktop\Projects\MapMyJIIT\BunkMyJIIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rushil\Desktop\Projects\BunkMyJIIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6239EC8B-E60D-4A85-A2CB-B234F08D75CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4437D9-6875-48EE-9670-3E2E98FF96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{68250A3F-BA9E-42BE-ABA5-2F7120A1BC65}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="169">
   <si>
     <t>ABB-I</t>
   </si>
@@ -538,13 +538,16 @@
   </si>
   <si>
     <t>MCL</t>
+  </si>
+  <si>
+    <t>ADC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +677,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -848,7 +858,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1023,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1345,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F85D740-A33C-469B-B8A8-5210F9C03359}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2602,44 +2615,44 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="29" t="s">
+      <c r="A114" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B114" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C114" s="13" t="s">
+      <c r="B114" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="50" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B115" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C115" s="13" t="s">
+      <c r="A115" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="50" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B116" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>156</v>
@@ -2647,51 +2660,51 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>33</v>
+        <v>156</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B122" s="30" t="s">
         <v>2</v>
@@ -2701,19 +2714,19 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B123" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>56</v>
+      <c r="A123" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B124" s="33" t="s">
         <v>55</v>
@@ -2724,73 +2737,73 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B125" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C125" s="13" t="s">
-        <v>158</v>
+        <v>55</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B126" s="33" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>1</v>
+        <v>158</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B127" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B127" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C127" s="13" t="s">
+      <c r="B128" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128" s="13" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B128" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C128" s="13" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B131" s="30" t="s">
         <v>19</v>
@@ -2801,7 +2814,7 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="30" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="B132" s="30" t="s">
         <v>19</v>
@@ -2812,7 +2825,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="30" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="B133" s="30" t="s">
         <v>19</v>
@@ -2823,29 +2836,29 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B134" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B134" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C134" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B135" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C135" s="50" t="s">
+      <c r="B135" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="49" t="s">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="B136" s="49" t="s">
         <v>19</v>
@@ -2855,19 +2868,19 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B137" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C137" s="16" t="s">
-        <v>155</v>
+      <c r="A137" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" s="50" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B138" s="35" t="s">
         <v>0</v>
@@ -2878,7 +2891,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B139" s="35" t="s">
         <v>0</v>
@@ -2889,7 +2902,7 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B140" s="35" t="s">
         <v>0</v>
@@ -2900,7 +2913,7 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B141" s="35" t="s">
         <v>0</v>
@@ -2911,7 +2924,7 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="34" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="B142" s="35" t="s">
         <v>0</v>
@@ -2921,19 +2934,19 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="B143" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C143" s="57" t="s">
-        <v>158</v>
+      <c r="A143" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B143" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="55" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B144" s="56" t="s">
         <v>19</v>
@@ -2943,68 +2956,79 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="36" t="s">
+      <c r="A145" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B145" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="57" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B145" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C145" s="45" t="s">
+      <c r="B146" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="34" t="s">
+    <row r="147" spans="1:3">
+      <c r="A147" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B146" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C146" s="16" t="s">
+      <c r="B147" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="38" t="s">
+    <row r="148" spans="1:3">
+      <c r="A148" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B147" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B148" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C148" s="13" t="s">
+      <c r="B148" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" s="46" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B149" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="51" t="s">
+      <c r="B150" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="B150" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="16" t="s">
+      <c r="B151" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="16" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: slight discrepancy with BT2&3
</commit_message>
<xml_diff>
--- a/RoomLocation.xlsx
+++ b/RoomLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rushil\Desktop\Projects\BunkMyJIIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4437D9-6875-48EE-9670-3E2E98FF96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDBEC83-96AA-424D-8A70-2CE40A247EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{68250A3F-BA9E-42BE-ABA5-2F7120A1BC65}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="170">
   <si>
     <t>ABB-I</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>ADC</t>
+  </si>
+  <si>
+    <t>BT2&amp;3</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1036,6 +1039,15 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1358,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F85D740-A33C-469B-B8A8-5210F9C03359}">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2934,30 +2946,30 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="34" t="s">
+      <c r="A143" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="B143" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" s="62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B143" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C143" s="16" t="s">
+      <c r="B144" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" s="16" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="B144" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C144" s="57" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="55" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B145" s="56" t="s">
         <v>19</v>
@@ -2967,68 +2979,79 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="36" t="s">
+      <c r="A146" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B146" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" s="57" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B146" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C146" s="45" t="s">
+      <c r="B147" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="34" t="s">
+    <row r="148" spans="1:3">
+      <c r="A148" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B147" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="16" t="s">
+      <c r="B148" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="38" t="s">
+    <row r="149" spans="1:3">
+      <c r="A149" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B148" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C148" s="46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B149" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C149" s="13" t="s">
+      <c r="B149" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" s="46" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B150" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="51" t="s">
+      <c r="B151" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="B151" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="16" t="s">
+      <c r="B152" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="16" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>